<commit_message>
Fixed UTF-8 apostrophe's from Excel auto-correct settings!!
</commit_message>
<xml_diff>
--- a/rfid_reader/data/FIRST Attendance - RFID tags.xlsx
+++ b/rfid_reader/data/FIRST Attendance - RFID tags.xlsx
@@ -475,9 +475,6 @@
     <t>Welcome other Jared</t>
   </si>
   <si>
-    <t>I'll miss you, other Jared…</t>
-  </si>
-  <si>
     <t>If you can dream it, you can do it.</t>
   </si>
   <si>
@@ -532,9 +529,6 @@
     <t>You go girl!</t>
   </si>
   <si>
-    <t xml:space="preserve">Being positive in a negative situation is not naïve. It's leadership. </t>
-  </si>
-  <si>
     <t xml:space="preserve">I never dreamed about success. I worked for it. </t>
   </si>
   <si>
@@ -565,9 +559,6 @@
     <t>I didn't come this far to only come this far.</t>
   </si>
   <si>
-    <t>Don’t' underestimate the power of coffee and a girl with a dream..</t>
-  </si>
-  <si>
     <t>I should probably kick some ass today</t>
   </si>
   <si>
@@ -589,9 +580,6 @@
     <t>A little progress each day adds up</t>
   </si>
   <si>
-    <t>You can stay but your clothes must go…</t>
-  </si>
-  <si>
     <t>You will never have this day again. Make it count.</t>
   </si>
   <si>
@@ -616,9 +604,6 @@
     <t>If not now, when?</t>
   </si>
   <si>
-    <t>Your only limit is you…</t>
-  </si>
-  <si>
     <t>You will kick ass today</t>
   </si>
   <si>
@@ -658,24 +643,12 @@
     <t>There are no goodbyes for us. Wherever you are, you will always be in my heart.</t>
   </si>
   <si>
-    <t>If you’re brave enough to say goodbye, life will reward you with a new hello.</t>
-  </si>
-  <si>
     <t>This is not a goodbye, my darling, this is a thank you.</t>
   </si>
   <si>
-    <t>Don’t cry because it’s over, smile because it happened.</t>
-  </si>
-  <si>
-    <t>Man’s feelings are always purest and most glowing in the hour of meeting and of farewell.</t>
-  </si>
-  <si>
     <t>Great is the art of beginning, but greater is the art of ending.</t>
   </si>
   <si>
-    <t>Goodbyes make you think. They make you realize what you’ve had, what you’ve lost, and what you’ve taken for granted.</t>
-  </si>
-  <si>
     <t>The pain of parting is nothing to the joy of meeting again.</t>
   </si>
   <si>
@@ -694,21 +667,9 @@
     <t>Despite my ghoulish reputation, I really have the heart of a small boy. I keep it in a jar on my desk.</t>
   </si>
   <si>
-    <t xml:space="preserve">Go confidently in the direction of your dreams. Lof the life you've imagined.  </t>
-  </si>
-  <si>
     <t xml:space="preserve">It takes courage to lef go of the familiar and embrace the new. </t>
   </si>
   <si>
-    <t>How lucky I am to have something that makes saying goodby so hard…</t>
-  </si>
-  <si>
-    <t>You may be far from my sight but you are never gone from my heart…</t>
-  </si>
-  <si>
-    <t>I started missing you as soon as you signed out…</t>
-  </si>
-  <si>
     <t>Someday you'll see the reason there is Good in goodbye</t>
   </si>
   <si>
@@ -721,9 +682,6 @@
     <t>You'll never be bored when you try soemething new. There's really no limit to what you can do!</t>
   </si>
   <si>
-    <t>He asked my favorite position. I said "CEO". And then I broke his arm…</t>
-  </si>
-  <si>
     <t>Why fit it when you are born to stand out?</t>
   </si>
   <si>
@@ -742,22 +700,13 @@
     <t>A person is a person, no matter how small! Dr. Seuss</t>
   </si>
   <si>
-    <t>Isn't it funny how day by day nothing changes but when you look back everhting is different…</t>
-  </si>
-  <si>
     <t>And will you succeed? Yes! You will indeed (98 and 3/4 percent) guaranteed!</t>
   </si>
   <si>
     <t xml:space="preserve">You're off to great places, today is your day, your mountain is waiting, so get on your way. </t>
   </si>
   <si>
-    <t>A photograph is the pause button of life…</t>
-  </si>
-  <si>
     <t>It's better to know how to learn than to know</t>
-  </si>
-  <si>
-    <t>All that awesome is such a little boy…</t>
   </si>
   <si>
     <t>You only live once. Might as well be a badass!</t>
@@ -791,22 +740,73 @@
 4) Nice butt</t>
   </si>
   <si>
-    <t>We’ll meet again, 
-Don’t know where,don’t know when, 
-But I know we’ll meet again, some sunny day.</t>
+    <t>Man's feelings are always purest and most glowing in the hour of meeting and of farewell.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Go confidently in the direction of your dreams. Live the life you've imagined.  </t>
+  </si>
+  <si>
+    <t>If you're brave enough to say goodbye, life will reward you with a new hello.</t>
+  </si>
+  <si>
+    <t>Don't underestimate the power of coffee and a girl with a dream..</t>
+  </si>
+  <si>
+    <t>A photograph is the pause button of life...</t>
+  </si>
+  <si>
+    <t>I'll miss you, other Jared...</t>
+  </si>
+  <si>
+    <t>How lucky I am to have something that makes saying goodby so hard...</t>
+  </si>
+  <si>
+    <t>You may be far from my sight but you are never gone from my heart...</t>
+  </si>
+  <si>
+    <t>I started missing you as soon as you signed out...</t>
+  </si>
+  <si>
+    <t>He asked my favorite position. I said "CEO". And then I broke his arm...</t>
+  </si>
+  <si>
+    <t>Your only limit is you...</t>
+  </si>
+  <si>
+    <t>Isn't it funny how day by day nothing changes but when you look back everhting is different...</t>
+  </si>
+  <si>
+    <t>You can stay but your clothes must go...</t>
+  </si>
+  <si>
+    <t>All that awesome is such a little boy...</t>
   </si>
   <si>
     <t>Goodbyes are not forever, 
 Goodbyes are not the end. 
-They simply mean I’ll miss you, 
+They simply mean I'll miss you, 
 Until we meet again.</t>
   </si>
   <si>
-    <t>One, two, Freddy’s coming for you.  
+    <t>Don't cry because it's over, smile because it happened.</t>
+  </si>
+  <si>
+    <t>We'll meet again, 
+Don't know where,Don't know when, 
+But I know we’ll meet again, some sunny day.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Being positive in a negative situation is not naive. It's leadership. </t>
+  </si>
+  <si>
+    <t>One, two, Freddy's coming for you.  
 Three, four, better lock your door. 
 Five, six, grab your crucifix. 
 Seven, eight, gonna stay up late. 
 Nine, ten, never sleep again.</t>
+  </si>
+  <si>
+    <t>Goodbyes make you think. They make you realize what you've had, what you've lost, and what you've taken for granted.</t>
   </si>
 </sst>
 </file>
@@ -1251,9 +1251,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1300,10 +1300,10 @@
         <v>33</v>
       </c>
       <c r="C3" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="D3" s="15" t="s">
         <v>148</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="12.75">
@@ -1314,10 +1314,10 @@
         <v>133</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="12.75">
@@ -1328,10 +1328,10 @@
         <v>32</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="12.75">
@@ -1342,10 +1342,10 @@
         <v>34</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="12.75">
@@ -1356,10 +1356,10 @@
         <v>134</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="12.75">
@@ -1370,10 +1370,10 @@
         <v>135</v>
       </c>
       <c r="C8" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="D8" s="15" t="s">
         <v>146</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="12.75">
@@ -1384,10 +1384,10 @@
         <v>136</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="12.75">
@@ -1430,10 +1430,10 @@
         <v>10</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15">
@@ -1444,10 +1444,10 @@
         <v>16</v>
       </c>
       <c r="C16" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>194</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="12.75">
@@ -1458,10 +1458,10 @@
         <v>111</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="12.75">
@@ -1472,10 +1472,10 @@
         <v>26</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>213</v>
+        <v>228</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="12.75">
@@ -1486,10 +1486,10 @@
         <v>9</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="12.75">
@@ -1500,10 +1500,10 @@
         <v>22</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>201</v>
+        <v>190</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="12.75">
@@ -1516,8 +1516,8 @@
       <c r="C21" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="D21" s="8" t="s">
-        <v>203</v>
+      <c r="D21" s="6" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="12.75">
@@ -1528,10 +1528,10 @@
         <v>19</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="63.75">
@@ -1542,10 +1542,10 @@
         <v>29</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>243</v>
+        <v>226</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>242</v>
+        <v>225</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="12.75">
@@ -1556,10 +1556,10 @@
         <v>23</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>204</v>
+        <v>187</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.25">
@@ -1570,10 +1570,10 @@
         <v>113</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="51">
@@ -1584,10 +1584,10 @@
         <v>114</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="12.75">
@@ -1598,10 +1598,10 @@
         <v>18</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>206</v>
+        <v>186</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="12.75">
@@ -1615,7 +1615,7 @@
         <v>137</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="12.75">
@@ -1629,7 +1629,7 @@
         <v>139</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>140</v>
+        <v>232</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="12.75">
@@ -1640,10 +1640,10 @@
         <v>116</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="12.75">
@@ -1654,10 +1654,10 @@
         <v>117</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="12.75">
@@ -1668,10 +1668,10 @@
         <v>5</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="12.75">
@@ -1682,10 +1682,10 @@
         <v>24</v>
       </c>
       <c r="C33" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="D33" s="6" t="s">
         <v>198</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="51">
@@ -1696,10 +1696,10 @@
         <v>15</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="12.75">
@@ -1710,10 +1710,10 @@
         <v>118</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>215</v>
+        <v>233</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="12.75">
@@ -1724,10 +1724,10 @@
         <v>119</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>216</v>
+        <v>234</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="12.75">
@@ -1738,10 +1738,10 @@
         <v>14</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>217</v>
+        <v>235</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="12.75">
@@ -1752,10 +1752,10 @@
         <v>120</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="12.75">
@@ -1766,10 +1766,10 @@
         <v>30</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>170</v>
+        <v>230</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="12.75">
@@ -1780,10 +1780,10 @@
         <v>12</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="12.75">
@@ -1794,10 +1794,10 @@
         <v>31</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="12.75">
@@ -1808,10 +1808,10 @@
         <v>121</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="12.75">
@@ -1822,10 +1822,10 @@
         <v>122</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>222</v>
+        <v>236</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="12.75">
@@ -1836,10 +1836,10 @@
         <v>123</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="12.75">
@@ -1850,10 +1850,10 @@
         <v>124</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="12.75">
@@ -1867,7 +1867,7 @@
         <v>139</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>140</v>
+        <v>232</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="12.75">
@@ -1878,10 +1878,10 @@
         <v>6</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="12.75">
@@ -1892,10 +1892,10 @@
         <v>20</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="12.75">
@@ -1906,10 +1906,10 @@
         <v>126</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="12.75">
@@ -1920,10 +1920,10 @@
         <v>125</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="12.75">
@@ -1934,10 +1934,10 @@
         <v>25</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>187</v>
+        <v>237</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="12.75">
@@ -1948,10 +1948,10 @@
         <v>8</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="12.75">
@@ -1962,10 +1962,10 @@
         <v>127</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D53" s="15" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="12.75">
@@ -1976,10 +1976,10 @@
         <v>21</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>229</v>
+        <v>238</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="12.75">
@@ -1990,10 +1990,10 @@
         <v>17</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="12.75">
@@ -2004,10 +2004,10 @@
         <v>128</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="63.75">
@@ -2018,10 +2018,10 @@
         <v>7</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="D57" s="16" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="12.75">
@@ -2032,10 +2032,10 @@
         <v>129</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="12.75">
@@ -2046,10 +2046,10 @@
         <v>13</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>178</v>
+        <v>239</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="12.75">
@@ -2060,10 +2060,10 @@
         <v>130</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="12.75">
@@ -2074,10 +2074,10 @@
         <v>131</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>235</v>
+        <v>218</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="12.75">
@@ -2088,10 +2088,10 @@
         <v>11</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>239</v>
+        <v>222</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="12.75">
@@ -2102,10 +2102,10 @@
         <v>132</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>236</v>
+        <v>219</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="12.75">
@@ -2114,7 +2114,7 @@
       </c>
       <c r="B64" s="9"/>
       <c r="C64" s="3" t="s">
-        <v>237</v>
+        <v>220</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="15.75" customHeight="1">

</xml_diff>